<commit_message>
Changed SQL query function
Query's are now written dynamically so that only one select function is
necessary.
</commit_message>
<xml_diff>
--- a/TimeLog.xlsx
+++ b/TimeLog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>added OpenFileDialog control and have system reading in the CSV files; Nothing happens with data yet</t>
+  </si>
+  <si>
+    <t>Redesigned Query function,</t>
   </si>
 </sst>
 </file>
@@ -417,7 +420,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G344"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -476,7 +479,7 @@
       </c>
       <c r="G2" s="7">
         <f>SUM(F2:F1000)</f>
-        <v>0.26041666666666674</v>
+        <v>-0.28124999999999989</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -543,7 +546,22 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F6" s="3"/>
+      <c r="A6" s="1">
+        <v>41773</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="3">
+        <f xml:space="preserve"> C6 - B6</f>
+        <v>-0.54166666666666663</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F7" s="3"/>

</xml_diff>

<commit_message>
Tech Query Completed & DGV working
Completed Query for Technicians and DGV now working
</commit_message>
<xml_diff>
--- a/TimeLog.xlsx
+++ b/TimeLog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>Date</t>
   </si>
@@ -81,13 +81,23 @@
   </si>
   <si>
     <t>Finished importing activities</t>
+  </si>
+  <si>
+    <t>Finished constructing sql query for tech search and added datagridview; dgv not operational yet.</t>
+  </si>
+  <si>
+    <t>Joey's Pay</t>
+  </si>
+  <si>
+    <t>DGV now operational.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
     <numFmt numFmtId="165" formatCode="h:mm;@"/>
   </numFmts>
@@ -143,7 +153,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1"/>
@@ -152,6 +162,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -433,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G344"/>
+  <dimension ref="A1:H344"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,9 +458,10 @@
     <col min="4" max="4" width="18.42578125" customWidth="1"/>
     <col min="5" max="5" width="110" customWidth="1"/>
     <col min="7" max="7" width="14.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -471,8 +483,11 @@
       <c r="G1" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="H1" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>41768</v>
       </c>
@@ -494,10 +509,10 @@
       </c>
       <c r="G2" s="7">
         <f>SUM(F2:F1000)</f>
-        <v>0.8125</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.9375</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>41768</v>
       </c>
@@ -518,7 +533,7 @@
         <v>4.166666666666663E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>41771</v>
       </c>
@@ -539,7 +554,7 @@
         <v>0.10416666666666663</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>41773</v>
       </c>
@@ -560,7 +575,7 @@
         <v>8.333333333333337E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>41773</v>
       </c>
@@ -581,7 +596,7 @@
         <v>0.14583333333333337</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>41774</v>
       </c>
@@ -602,7 +617,7 @@
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>41774</v>
       </c>
@@ -623,7 +638,7 @@
         <v>8.3333333333333259E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>41775</v>
       </c>
@@ -644,7 +659,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>41775</v>
       </c>
@@ -665,22 +680,61 @@
         <v>0.12500000000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>41775</v>
+      </c>
+      <c r="B11" s="5">
+        <v>0.5625</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0.625</v>
+      </c>
+      <c r="D11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="3">
+        <f xml:space="preserve"> C11 - B11</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="H11" s="8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>41775</v>
+      </c>
+      <c r="B12" s="5">
+        <v>0.6875</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="D12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="3">
+        <f xml:space="preserve"> C12 - B12</f>
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F16" s="3"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added Sort and progress bar to form
</commit_message>
<xml_diff>
--- a/TimeLog.xlsx
+++ b/TimeLog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>Date</t>
   </si>
@@ -450,7 +450,7 @@
   <dimension ref="A1:H344"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,7 +508,7 @@
         <v>8</v>
       </c>
       <c r="F2" s="3">
-        <f xml:space="preserve"> C2 - B2</f>
+        <f t="shared" ref="F2:F12" si="0" xml:space="preserve"> C2 - B2</f>
         <v>4.1666666666666741E-2</v>
       </c>
       <c r="G2" s="7">
@@ -533,7 +533,7 @@
         <v>7</v>
       </c>
       <c r="F3" s="3">
-        <f xml:space="preserve"> C3 - B3</f>
+        <f t="shared" si="0"/>
         <v>4.166666666666663E-2</v>
       </c>
     </row>
@@ -554,7 +554,7 @@
         <v>9</v>
       </c>
       <c r="F4" s="3">
-        <f xml:space="preserve"> C4 - B4</f>
+        <f t="shared" si="0"/>
         <v>0.10416666666666663</v>
       </c>
     </row>
@@ -575,7 +575,7 @@
         <v>12</v>
       </c>
       <c r="F5" s="3">
-        <f xml:space="preserve"> C5 - B5</f>
+        <f t="shared" si="0"/>
         <v>8.333333333333337E-2</v>
       </c>
     </row>
@@ -596,7 +596,7 @@
         <v>14</v>
       </c>
       <c r="F6" s="3">
-        <f xml:space="preserve"> C6 - B6</f>
+        <f t="shared" si="0"/>
         <v>0.14583333333333337</v>
       </c>
     </row>
@@ -617,7 +617,7 @@
         <v>15</v>
       </c>
       <c r="F7" s="3">
-        <f xml:space="preserve"> C7 - B7</f>
+        <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
     </row>
@@ -638,7 +638,7 @@
         <v>16</v>
       </c>
       <c r="F8" s="3">
-        <f xml:space="preserve"> C8 - B8</f>
+        <f t="shared" si="0"/>
         <v>8.3333333333333259E-2</v>
       </c>
     </row>
@@ -659,7 +659,7 @@
         <v>17</v>
       </c>
       <c r="F9" s="3">
-        <f xml:space="preserve"> C9 - B9</f>
+        <f t="shared" si="0"/>
         <v>0.125</v>
       </c>
     </row>
@@ -680,7 +680,7 @@
         <v>18</v>
       </c>
       <c r="F10" s="3">
-        <f xml:space="preserve"> C10 - B10</f>
+        <f t="shared" si="0"/>
         <v>0.12500000000000003</v>
       </c>
     </row>
@@ -701,7 +701,7 @@
         <v>19</v>
       </c>
       <c r="F11" s="3">
-        <f xml:space="preserve"> C11 - B11</f>
+        <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
       <c r="H11" s="8" t="s">
@@ -725,11 +725,20 @@
         <v>22</v>
       </c>
       <c r="F12" s="3">
-        <f xml:space="preserve"> C12 - B12</f>
+        <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>41778</v>
+      </c>
+      <c r="B13" s="5">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
finished calculations and meet with heath
</commit_message>
<xml_diff>
--- a/TimeLog.xlsx
+++ b/TimeLog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -93,16 +93,20 @@
   </si>
   <si>
     <t>DGV now operational. And Total is calculated</t>
+  </si>
+  <si>
+    <t>Fixed Calculations</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
     <numFmt numFmtId="165" formatCode="h:mm;@"/>
+    <numFmt numFmtId="167" formatCode="[h]:mm:ss;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -156,7 +160,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1"/>
@@ -166,6 +170,7 @@
     <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -449,8 +454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H344"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,12 +513,12 @@
         <v>8</v>
       </c>
       <c r="F2" s="3">
-        <f t="shared" ref="F2:F12" si="0" xml:space="preserve"> C2 - B2</f>
+        <f t="shared" ref="F2:F13" si="0" xml:space="preserve"> C2 - B2</f>
         <v>4.1666666666666741E-2</v>
       </c>
-      <c r="G2" s="7">
-        <f>SUM(F2:F1000)</f>
-        <v>0.9375</v>
+      <c r="G2" s="9">
+        <f>SUM(F2:F100)</f>
+        <v>1.0416666666666665</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -736,10 +741,19 @@
       <c r="B13" s="5">
         <v>0.29166666666666669</v>
       </c>
+      <c r="C13" s="5">
+        <v>0.39583333333333331</v>
+      </c>
       <c r="D13" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="3"/>
+      <c r="E13" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="3">
+        <f t="shared" si="0"/>
+        <v>0.10416666666666663</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F14" s="3"/>

</xml_diff>

<commit_message>
Test Files; Receivers now import; tweeked GUI
Added open file dialog title change
Receivers now import correctly
Test Files were moved into folder
</commit_message>
<xml_diff>
--- a/TimeLog.xlsx
+++ b/TimeLog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
   <si>
     <t>Date</t>
   </si>
@@ -461,7 +461,7 @@
   <dimension ref="A1:H344"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,12 +519,12 @@
         <v>8</v>
       </c>
       <c r="F2" s="3">
-        <f t="shared" ref="F2:F15" si="0" xml:space="preserve"> C2 - B2</f>
+        <f t="shared" ref="F2:F16" si="0" xml:space="preserve"> C2 - B2</f>
         <v>4.1666666666666741E-2</v>
       </c>
       <c r="G2" s="9">
         <f>SUM(F2:F100)</f>
-        <v>1.1354166666666665</v>
+        <v>1.177083333333333</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -804,7 +804,22 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F16" s="3"/>
+      <c r="A16" s="1">
+        <v>41781</v>
+      </c>
+      <c r="B16" s="5">
+        <v>0.95763888888888893</v>
+      </c>
+      <c r="C16" s="5">
+        <v>0.99930555555555556</v>
+      </c>
+      <c r="D16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="3">
+        <f t="shared" si="0"/>
+        <v>4.166666666666663E-2</v>
+      </c>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F17" s="3"/>

</xml_diff>

<commit_message>
Commenting code & timestamp
</commit_message>
<xml_diff>
--- a/TimeLog.xlsx
+++ b/TimeLog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
   <si>
     <t>Date</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>Added paid column, need to complete abilty to pay off</t>
+  </si>
+  <si>
+    <t>Imported Receivers and completed pay.</t>
   </si>
 </sst>
 </file>
@@ -460,8 +463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H344"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,7 +527,7 @@
       </c>
       <c r="G2" s="9">
         <f>SUM(F2:F100)</f>
-        <v>1.177083333333333</v>
+        <v>1.2916666666666663</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -787,7 +790,7 @@
         <v>41781</v>
       </c>
       <c r="B15" s="5">
-        <v>0.65625</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="C15" s="5">
         <v>0.6875</v>
@@ -800,25 +803,28 @@
       </c>
       <c r="F15" s="3">
         <f t="shared" si="0"/>
-        <v>3.125E-2</v>
+        <v>4.166666666666663E-2</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>41781</v>
+        <v>41782</v>
       </c>
       <c r="B16" s="5">
-        <v>0.95763888888888893</v>
+        <v>0</v>
       </c>
       <c r="C16" s="5">
-        <v>0.99930555555555556</v>
+        <v>0.14583333333333334</v>
       </c>
       <c r="D16" t="s">
         <v>13</v>
       </c>
+      <c r="E16" t="s">
+        <v>26</v>
+      </c>
       <c r="F16" s="3">
         <f t="shared" si="0"/>
-        <v>4.166666666666663E-2</v>
+        <v>0.14583333333333334</v>
       </c>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Name Change and SQL Fix
Serial was changed to serialnum in query
</commit_message>
<xml_diff>
--- a/TimeLog.xlsx
+++ b/TimeLog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>Imported Receivers and completed pay.</t>
+  </si>
+  <si>
+    <t>Adde RecInv dgv and created query for it.</t>
   </si>
 </sst>
 </file>
@@ -115,7 +118,7 @@
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="164" formatCode="[$-409]h:mm\ AM/PM;@"/>
     <numFmt numFmtId="165" formatCode="h:mm;@"/>
-    <numFmt numFmtId="167" formatCode="[h]:mm:ss;@"/>
+    <numFmt numFmtId="166" formatCode="[h]:mm:ss;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -179,7 +182,7 @@
     <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -463,8 +466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H344"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,12 +525,12 @@
         <v>8</v>
       </c>
       <c r="F2" s="3">
-        <f t="shared" ref="F2:F16" si="0" xml:space="preserve"> C2 - B2</f>
+        <f t="shared" ref="F2:F17" si="0" xml:space="preserve"> C2 - B2</f>
         <v>4.1666666666666741E-2</v>
       </c>
       <c r="G2" s="9">
         <f>SUM(F2:F100)</f>
-        <v>1.2916666666666663</v>
+        <v>1.3541666666666663</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -827,52 +830,67 @@
         <v>0.14583333333333334</v>
       </c>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="5">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C17" s="5">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" s="3">
+        <f t="shared" si="0"/>
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F32" s="3"/>
     </row>
     <row r="33" spans="6:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Transfer Receiver filling Fields 1.0
Transfer Receiver Fields retrieves serial scanned by user and searches
for the previous owner of the receiver. So far sql retrieval of owner is
done. now to fill the textbox with result.
</commit_message>
<xml_diff>
--- a/TimeLog.xlsx
+++ b/TimeLog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
   <si>
     <t>Date</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>Adde RecInv dgv and created query for it.</t>
+  </si>
+  <si>
+    <t>(M4.5;W4;F5)$135/$135</t>
   </si>
 </sst>
 </file>
@@ -467,7 +470,7 @@
   <dimension ref="A1:H344"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,7 +481,7 @@
     <col min="4" max="4" width="18.42578125" customWidth="1"/>
     <col min="5" max="5" width="97.140625" customWidth="1"/>
     <col min="7" max="7" width="14.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" customWidth="1"/>
     <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -830,7 +833,10 @@
         <v>0.14583333333333334</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>41782</v>
+      </c>
       <c r="B17" s="5">
         <v>0.54166666666666663</v>
       </c>
@@ -847,50 +853,53 @@
         <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F32" s="3"/>
     </row>
     <row r="33" spans="6:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Text Search, Receivers transfer, Payment recording
a large update that should have been committed more often but wasn't so
your stuck with all that in one.
</commit_message>
<xml_diff>
--- a/TimeLog.xlsx
+++ b/TimeLog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
   <si>
     <t>Date</t>
   </si>
@@ -111,6 +111,12 @@
   </si>
   <si>
     <t>(M4.5;W4;F5)$135/$135</t>
+  </si>
+  <si>
+    <t>Restructure of search method.</t>
+  </si>
+  <si>
+    <t>Finished restructuring search method, added extra tabs and tables, added transfer of receivers.</t>
   </si>
 </sst>
 </file>
@@ -470,7 +476,7 @@
   <dimension ref="A1:H344"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,12 +534,12 @@
         <v>8</v>
       </c>
       <c r="F2" s="3">
-        <f t="shared" ref="F2:F17" si="0" xml:space="preserve"> C2 - B2</f>
+        <f t="shared" ref="F2:F19" si="0" xml:space="preserve"> C2 - B2</f>
         <v>4.1666666666666741E-2</v>
       </c>
       <c r="G2" s="9">
         <f>SUM(F2:F100)</f>
-        <v>1.3541666666666663</v>
+        <v>1.708333333333333</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -858,10 +864,46 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F18" s="3"/>
+      <c r="A18" s="1">
+        <v>41786</v>
+      </c>
+      <c r="B18" s="5">
+        <v>0.95763888888888893</v>
+      </c>
+      <c r="C18" s="5">
+        <v>0.99930555555555556</v>
+      </c>
+      <c r="D18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="3">
+        <f t="shared" si="0"/>
+        <v>4.166666666666663E-2</v>
+      </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F19" s="3"/>
+      <c r="A19" s="1">
+        <v>41787</v>
+      </c>
+      <c r="B19" s="5">
+        <v>0</v>
+      </c>
+      <c r="C19" s="5">
+        <v>0.3125</v>
+      </c>
+      <c r="D19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="3">
+        <f t="shared" si="0"/>
+        <v>0.3125</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F20" s="3"/>

</xml_diff>

<commit_message>
Added techless search, Fixed DGV filter
DGV fix was performed by changing the column to a numerical field
instead of a nvarchar.
</commit_message>
<xml_diff>
--- a/TimeLog.xlsx
+++ b/TimeLog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
   <si>
     <t>Date</t>
   </si>
@@ -117,6 +117,12 @@
   </si>
   <si>
     <t>Finished restructuring search method, added extra tabs and tables, added transfer of receivers.</t>
+  </si>
+  <si>
+    <t>Added Techless searchs.</t>
+  </si>
+  <si>
+    <t>Fixed Format on Currency columns.</t>
   </si>
 </sst>
 </file>
@@ -476,7 +482,7 @@
   <dimension ref="A1:H344"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,12 +540,12 @@
         <v>8</v>
       </c>
       <c r="F2" s="3">
-        <f t="shared" ref="F2:F19" si="0" xml:space="preserve"> C2 - B2</f>
+        <f t="shared" ref="F2:F21" si="0" xml:space="preserve"> C2 - B2</f>
         <v>4.1666666666666741E-2</v>
       </c>
       <c r="G2" s="9">
         <f>SUM(F2:F100)</f>
-        <v>1.708333333333333</v>
+        <v>1.875</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -906,10 +912,46 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F20" s="3"/>
+      <c r="A20" s="1">
+        <v>41787</v>
+      </c>
+      <c r="B20" s="5">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C20" s="5">
+        <v>0.625</v>
+      </c>
+      <c r="D20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" s="3">
+        <f t="shared" si="0"/>
+        <v>8.333333333333337E-2</v>
+      </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F21" s="3"/>
+      <c r="A21" s="1">
+        <v>41787</v>
+      </c>
+      <c r="B21" s="5">
+        <v>0.625</v>
+      </c>
+      <c r="C21" s="5">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" s="3">
+        <f t="shared" si="0"/>
+        <v>8.333333333333337E-2</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F22" s="3"/>

</xml_diff>

<commit_message>
Progress Bar/Threading, File Printing, Program smoothing
</commit_message>
<xml_diff>
--- a/TimeLog.xlsx
+++ b/TimeLog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="35">
   <si>
     <t>Date</t>
   </si>
@@ -123,6 +123,12 @@
   </si>
   <si>
     <t>Fixed Format on Currency columns.</t>
+  </si>
+  <si>
+    <t>Worked on Threading Process Bar</t>
+  </si>
+  <si>
+    <t>Finished Progress bar, set up File to Print, Smoothed errors and visual appeal</t>
   </si>
 </sst>
 </file>
@@ -482,7 +488,7 @@
   <dimension ref="A1:H344"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,12 +546,12 @@
         <v>8</v>
       </c>
       <c r="F2" s="3">
-        <f t="shared" ref="F2:F21" si="0" xml:space="preserve"> C2 - B2</f>
+        <f t="shared" ref="F2:F23" si="0" xml:space="preserve"> C2 - B2</f>
         <v>4.1666666666666741E-2</v>
       </c>
       <c r="G2" s="9">
         <f>SUM(F2:F100)</f>
-        <v>1.875</v>
+        <v>2.2083333333333335</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -954,10 +960,46 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F22" s="3"/>
+      <c r="A22" s="1">
+        <v>41788</v>
+      </c>
+      <c r="B22" s="5">
+        <v>0.93680555555555556</v>
+      </c>
+      <c r="C22" s="5">
+        <v>0.99930555555555556</v>
+      </c>
+      <c r="D22" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" s="3">
+        <f t="shared" si="0"/>
+        <v>6.25E-2</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F23" s="3"/>
+      <c r="A23" s="1">
+        <v>41789</v>
+      </c>
+      <c r="B23" s="5">
+        <v>0</v>
+      </c>
+      <c r="C23" s="5">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="D23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23" s="3">
+        <f t="shared" si="0"/>
+        <v>0.27083333333333331</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F24" s="3"/>

</xml_diff>

<commit_message>
Added Check for duplicates
and worked on printer issues.
</commit_message>
<xml_diff>
--- a/TimeLog.xlsx
+++ b/TimeLog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
   <si>
     <t>Date</t>
   </si>
@@ -125,10 +125,7 @@
     <t>Fixed Format on Currency columns.</t>
   </si>
   <si>
-    <t>Worked on Threading Process Bar</t>
-  </si>
-  <si>
-    <t>Finished Progress bar, set up File to Print, Smoothed errors and visual appeal</t>
+    <t xml:space="preserve">Finished Progress bar threading, File Printing, General smoothing and added duplicacy Check. </t>
   </si>
 </sst>
 </file>
@@ -488,7 +485,7 @@
   <dimension ref="A1:H344"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,7 +548,7 @@
       </c>
       <c r="G2" s="9">
         <f>SUM(F2:F100)</f>
-        <v>2.2083333333333335</v>
+        <v>2.2291666666666665</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -961,13 +958,13 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>41788</v>
+        <v>41789</v>
       </c>
       <c r="B22" s="5">
-        <v>0.93680555555555556</v>
+        <v>0</v>
       </c>
       <c r="C22" s="5">
-        <v>0.99930555555555556</v>
+        <v>0.35416666666666669</v>
       </c>
       <c r="D22" t="s">
         <v>13</v>
@@ -977,29 +974,12 @@
       </c>
       <c r="F22" s="3">
         <f t="shared" si="0"/>
-        <v>6.25E-2</v>
+        <v>0.35416666666666669</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>41789</v>
-      </c>
-      <c r="B23" s="5">
-        <v>0</v>
-      </c>
-      <c r="C23" s="5">
-        <v>0.27083333333333331</v>
-      </c>
-      <c r="D23" t="s">
-        <v>13</v>
-      </c>
-      <c r="E23" t="s">
-        <v>34</v>
-      </c>
-      <c r="F23" s="3">
-        <f t="shared" si="0"/>
-        <v>0.27083333333333331</v>
-      </c>
+      <c r="A23" s="1"/>
+      <c r="F23" s="3"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F24" s="3"/>

</xml_diff>